<commit_message>
Added basic code to main.py
</commit_message>
<xml_diff>
--- a/exclude/user-signedup_task-traker.xlsx
+++ b/exclude/user-signedup_task-traker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lc101\user-signup\exclude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A6D62C9-6E9F-4536-881F-E9615BADC122}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561C14D-BEED-466C-A7BB-B32A211A4F3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6084" xr2:uid="{C07FD9D2-63CD-4FAD-A76A-2B404D6040BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>user_signup task checklist</t>
   </si>
@@ -45,7 +45,28 @@
     <t>add .</t>
   </si>
   <si>
-    <t xml:space="preserve">created </t>
+    <t>create github repo &amp; .gitignore</t>
+  </si>
+  <si>
+    <t>create exclude folder &amp; added to .gitignore</t>
+  </si>
+  <si>
+    <t>create template folder &amp; main.py</t>
+  </si>
+  <si>
+    <t>pull master</t>
+  </si>
+  <si>
+    <t>activate flask-env</t>
+  </si>
+  <si>
+    <t>mofify .gitignore add .vscode and exclude folder</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -81,8 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,24 +422,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617ED22B-4F79-4E31-8007-F3726DB57353}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.21875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -426,16 +454,114 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43440</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creted css files and html base template
</commit_message>
<xml_diff>
--- a/exclude/user-signedup_task-traker.xlsx
+++ b/exclude/user-signedup_task-traker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lc101\user-signup\exclude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1425566A-190A-4DA6-A9D4-986857A1109A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E15FC1A-CFD3-4262-9624-FBA7DAFB8CDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6084" xr2:uid="{C07FD9D2-63CD-4FAD-A76A-2B404D6040BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>user_signup task checklist</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submission is not valid, reject it and re-render </t>
+  </si>
+  <si>
+    <t xml:space="preserve">feedback message should be next to the field </t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617ED22B-4F79-4E31-8007-F3726DB57353}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,6 +566,16 @@
         <v>43440</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>